<commit_message>
jira issues cleansing - all arabic excel file
</commit_message>
<xml_diff>
--- a/jira-issues/data/Etisalat Jira 2019-05-23T11_54_29+0400-ar-clean.xlsx
+++ b/jira-issues/data/Etisalat Jira 2019-05-23T11_54_29+0400-ar-clean.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="1200">
   <si>
     <t xml:space="preserve">Issue key</t>
   </si>
@@ -28012,7 +28012,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> خياط نعيم رياض نعيم </t>
+    <t xml:space="preserve"> خياط نعيم</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-587</t>
@@ -28192,7 +28192,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> صيدلية العين ثلثمية العين</t>
+    <t xml:space="preserve"> صيدلية العين</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-586</t>
@@ -28482,7 +28482,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> الراعي بانياس الرأي في بانياس </t>
+    <t xml:space="preserve"> الراعي بانياس</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-584</t>
@@ -28609,7 +28609,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كنتاكي الديك</t>
+    <t xml:space="preserve"> كنتاكي </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-579</t>
@@ -28799,7 +28799,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفي هيلث بيوينت مستشفى الفطيم</t>
+    <t xml:space="preserve"> مستشفي هيلث بيوينت</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-578</t>
@@ -28986,7 +28986,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كيف لاند مستشفى كيبل آند </t>
+    <t xml:space="preserve"> كيف لاند </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-567</t>
@@ -29122,7 +29122,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> طيران الإمارات الجعفرية </t>
+    <t xml:space="preserve"> طيران الإمارات  </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-561</t>
@@ -29209,7 +29209,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مكافأت مزيد مزيد</t>
+    <t xml:space="preserve"> مكافأت مزيد</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-555</t>
@@ -29296,7 +29296,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> سمايل ماي</t>
+    <t xml:space="preserve"> سمايل </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-550</t>
@@ -29470,51 +29470,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> ادنوك البطين</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-547</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested for "UAE RED CRESENT  " , VA recognised as "UAE connection"/recent"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 0e340ae14b15_016f09f0-3d90-11e9-ac7c-6f017d524293&lt;br&gt;
-EDUID: 5c7b92e5001300000a33a41423330002&lt;br&gt;
-Account Number: 0501204111&lt;br&gt;
-&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;customer requested for "UAE RED CRESENT&amp;nbsp; " , VA recognised as "UAE connection"/recent"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" _ngcontent-c21="" mat-table="" ng-reflect-data-source="[object Object],[object Object"&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c21="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;UAE connection&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;I didn't get that. Could you please specify the name of the place you are looking for?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;None&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;1&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c21="" mat-cell=""&gt;&amp;nbsp;&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c21="" mat-cell=""&gt;03/03/19 12:41:14 pm&lt;/td&gt;
-		&lt;/tr&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c21="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;recent&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;Looks like I couldn't help you here. I am connecting you to an advisor now.&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;Confirmation&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;0.8059&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c21="" mat-cell=""&gt;&amp;nbsp;&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c21="" mat-cell=""&gt;
-			&lt;p&gt;03/03/19 12:41:27 pm&lt;/p&gt;
-			&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-			&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> / </t>
+    <t xml:space="preserve"> ادنوك </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-542</t>
@@ -29714,7 +29670,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> نمره جامعة عجمان نمبر التى جمعت عجمان </t>
+    <t xml:space="preserve"> نمره جامعة عجمان</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-541</t>
@@ -29904,7 +29860,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> نمره جامعة عجمان نمرت يا جماعة عجمان </t>
+    <t xml:space="preserve"> نمره جامعة عجمان </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-538</t>
@@ -30069,7 +30025,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفي خليفة مستشف خليفة </t>
+    <t xml:space="preserve"> مستشفي خليفة </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-527</t>
@@ -30156,7 +30112,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> الفطيم للمشاريع التجارية الفطيم للمشاريع التجارية</t>
+    <t xml:space="preserve"> الفطيم للمشاريع التجارية </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-525</t>
@@ -30261,7 +30217,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> التيما لخدمات التنظيف الكرامة الفيمة والتنظيف</t>
+    <t xml:space="preserve"> التيما لخدمات التنظيف </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-524</t>
@@ -30366,7 +30322,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفى الكندي القير الكندي</t>
+    <t xml:space="preserve"> مستشفى الكندي</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-523</t>
@@ -30471,7 +30427,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مشاريع الشيراوى مقلية أم طائف الاوسط</t>
+    <t xml:space="preserve"> مشاريع الشيراوى</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-522</t>
@@ -30558,7 +30514,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> وندسور لتجارة المعدات الكهربائية وندسور لتجارة المعدات الكهربائية</t>
+    <t xml:space="preserve"> وندسور لتجارة المعدات الكهربائية</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-521</t>
@@ -30663,7 +30619,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> المجد لمواد البناء المجدل لمقاولات البناء المنزل لمقاولات البناء</t>
+    <t xml:space="preserve"> المجد لمواد البناء</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-520</t>
@@ -30750,7 +30706,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> بقالة التاج القرم</t>
+    <t xml:space="preserve"> بقالة التاج </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-519</t>
@@ -30855,7 +30811,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> شركة علي اكبر زماني التجارية شركة علي تعالي الزمان</t>
+    <t xml:space="preserve"> شركة علي اكبر زماني التجارية</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-518</t>
@@ -30960,7 +30916,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> الناصرة للالكترونيات الرحبة الله للالكترونيات</t>
+    <t xml:space="preserve"> الناصرة للالكترونيات</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-516</t>
@@ -31047,7 +31003,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> الاول للرياضة الأول</t>
+    <t xml:space="preserve"> الاول للرياضة</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-515</t>
@@ -31152,7 +31108,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> ماكدونالد ماكدونالد لا</t>
+    <t xml:space="preserve"> ماكدونالد</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-514</t>
@@ -31334,7 +31290,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كنتاكي منطقة الغرب </t>
+    <t xml:space="preserve"> كنتاكي</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-510</t>
@@ -31439,9 +31395,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> ماكدونالد ما دون ماك دونالد</t>
-  </si>
-  <si>
     <t xml:space="preserve">AVAT-508</t>
   </si>
   <si>
@@ -31562,7 +31515,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> فستفال مول بالمون دبي فستفال مول دبي فستفال سيتي</t>
+    <t xml:space="preserve"> فستفال مول</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-506</t>
@@ -31667,7 +31620,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> ميد كير أو مستشفى ميدكير متى كير مستشفى مدكير</t>
+    <t xml:space="preserve"> ميد كير</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-503</t>
@@ -31772,7 +31725,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مزيد مزيد </t>
+    <t xml:space="preserve"> مزيد  </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-502</t>
@@ -31925,7 +31878,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> 125 </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -32022,7 +31975,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مكافات مزيد الذيد</t>
+    <t xml:space="preserve"> مكافات مزيد </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-500</t>
@@ -32164,7 +32117,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> نقاط المزيد خدمة عملاء برستيج المقاطرة خدمة عملاء برستيج </t>
+    <t xml:space="preserve"> نقاط المزيد</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-498</t>
@@ -32346,7 +32299,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مخبزحلويات الخيام القير </t>
+    <t xml:space="preserve"> مخبز حلويات الخيام</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-496</t>
@@ -32528,7 +32481,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> فندق الشاطئ منطقة الشرق </t>
+    <t xml:space="preserve"> فندق الشاطئ </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-494</t>
@@ -32692,7 +32645,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> اسيا لتصنيع البراغيه نعم </t>
+    <t xml:space="preserve"> اسيا لتصنيع البراغيه</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-488</t>
@@ -32849,53 +32802,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> القنصلية السودانيه أحب كونستركشن</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-482</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VA did not recognize 'Jamil Optics' instead captured as 'main optics' &amp; jimmy optics for the 2nd trial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: d38a986b8a37_96eac9d0-34e7-11e9-9649-9943c4c18191&lt;br&gt;
-Conversation Status: completed&lt;br&gt;
-EDUID: 5c6d0c54002300000a33a41423330002&lt;br&gt;
-Account Number: 0501770990&lt;br&gt;
-&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" mat-table="" ng-reflect-data-source="[object Object],[object Object" _ngcontent-c13=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c13=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;main optics&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;Okay, so you would like to know the details of main optics right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;0.4401&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c13=""&gt;establishment: main optics&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c13=""&gt;20/02/19 12:14:50 pm&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VA did not capture and recognize the customer first 2 initial response      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div class="header" _ngcontent-c13=""&gt;
-&lt;div class="ng-star-inserted" _ngcontent-c13=""&gt;Conversation ID: 21e5cb925d6d_3db7e990-3c64-11e9-ac7c-6f017d524293&lt;br&gt;
-Conversation Status: completed&lt;br&gt;
-EDUID: 5c799c09000c00000a33a41423330002&lt;br&gt;
-Account Number: 0509979654&lt;br&gt;
-&amp;nbsp;&lt;/div&gt;
-&lt;div class="ng-star-inserted" _ngcontent-c13=""&gt;&amp;nbsp;&lt;/div&gt;
-&lt;div class="ng-star-inserted" _ngcontent-c13=""&gt;&amp;nbsp;&lt;/div&gt;
-&lt;/div&gt;
-</t>
+    <t xml:space="preserve"> القنصلية السودانيه </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-333</t>
@@ -32982,7 +32889,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> رقم اتصالات الطرفة</t>
+    <t xml:space="preserve"> رقم اتصالات </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-337</t>
@@ -33083,7 +32990,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> رقم كنتاكي ممكن يكبر </t>
+    <t xml:space="preserve"> رقم كنتاكي</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-378</t>
@@ -33339,35 +33246,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> شركة الفداء تربية </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "Light Touch ", VA recognised as "light Burj/light search"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 5386f0c36e0d_4ac3b6d0-34eb-11e9-b36c-47a9b5a11945&lt;br&gt;
-EDUID: 5c6d12a4001500000a33a41423330002&lt;br&gt;
-Account Number: 067037876&lt;/p&gt;
-&lt;p&gt;customer requested "Light Touch ", VA recognised as "light Burj/light search"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c13=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c13="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;I am looking for light Burj&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Okay, so you would like to know the details of light Burj right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;0.8221&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c13="" mat-cell=""&gt;establishment: light Burj&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c13="" mat-cell=""&gt;20/02/19 12:41:19 pm&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
+    <t xml:space="preserve"> شركة الفداء  </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-461</t>
@@ -33472,7 +33351,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفى راشد ايش راشد راشدال بل</t>
+    <t xml:space="preserve"> مستشفى راشد</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-459</t>
@@ -33559,7 +33438,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> رقم مزيد ابحث عن مكافآت مزيد </t>
+    <t xml:space="preserve"> رقم مزيد </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-453</t>
@@ -33646,182 +33525,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> أريد مطعم الظفره اريد مطعم البحار ظبي</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VA did not recognize nesrest Pizza hut instead captured as nearest Vega, customer repeated 2 times still did not capture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversation ID: 1da6036f97c0_a9d92c70-34e8-11e9-963b-758e7e407292
-Conversation Status: delegated
-EDUID: 5c6d0e3b000300000a33a41423330002
-Account Number: 0501114047
-VA did not recognize nesrest Pizza hut instead captured as nearest Vega, customer repeated 2 times still did not capture
-Give me the number of nearest Vega Okay, so you would like to know the details of Vega right? establishment_inquiry EstablishmentDetailsInquiry 0.9998 establishment: Vega 20/02/19 12:22:31 pm
-Nearest please I didn't get that. Could you please specify the name of the place you are looking for? establishment_inquiry EstablishmentDetailsInquiry 0.9673  20/02/19 12:22:53 pm
-visa Okay, so you would like to know the details of visa right? establishment_inquiry Confirmation 0.8572  20/02/19 12:23:08 pm
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-448</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Customer requirement:National corporation for tourism &amp; hotels system identified as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">أيمكنك </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">volition </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">الكورنيش الخجولة مكتوم</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Conversation:1da6036f97c0_58f132d0-34e8-11e9-b36c-47a9b5a11945
-EDUID:5c6d0da3000400000a33a41423330002
-Account Number: 0562002751
-Customer requirement:National corporation for tourism &amp; hotels
-system identified as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">أيمكنك </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">volition </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">الكورنيش الخجولة مكتوم
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> أيمكنك الكورنيش الخجولة مكتوم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-445</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "CROWN PRINCE", VA recognised as "hello Prince/Al Pirance"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 5386f0c36e0d_3739d020-34ed-11e9-8023-f9845d518eae&lt;br&gt;
-EDUID: 5c6d15de002500000a33a41423330002&lt;br&gt;
-Account Number: 0504457247&lt;/p&gt;
-&lt;p&gt;customer requested "CROWN PRINCE", VA recognised as "hello Prince/Al Pirance"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c13=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c13="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Al Pirance&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Okay, so you would like to know the details of Al Pirance right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;ChitChat.GreetSalam&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;0.3111&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c13="" mat-cell=""&gt;establishment: Al Pirance&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c13="" mat-cell=""&gt;
-			&lt;p&gt;20/02/19 12:55:21 pm&lt;/p&gt;
-			&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-			&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-440</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested " Paprika Restaurant", VA Entity recognised as "please call Cristal//paprika student"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 5386f0c36e0d_1962d8c0-34ee-11e9-b36c-47a9b5a11945&lt;br&gt;
-EDUID: 5c6d1754000400000a33a41423330002&lt;br&gt;
-Account Number: 0504462800&lt;br&gt;
-customer requested " Paprika Restaurant", VA Entity recognised as "please call Cristal//paprika student"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c13=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c13="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;please call Cristal&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Okay, so you would like to know the details of Cristal right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;0.4679&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c13="" mat-cell=""&gt;establishment: Cristal&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c13="" mat-cell=""&gt;20/02/19 1:01:37 pm&lt;/td&gt;
-		&lt;/tr&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c13="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;paprika student&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;The details of Cristal will be shared with you at the end of the call. Is this what you were looking for?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Confirmation&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;0.3713&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c13="" mat-cell=""&gt;establishment: paprika student&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c13="" mat-cell=""&gt;20/02/19 1:01:50 pm&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> // </t>
+    <t xml:space="preserve"> أريد مطعم الظفره</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-439</t>
@@ -33944,7 +33648,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> قصر الثقافة في الشارقة كي أف سي قصص قرى الشارقة كيف سين</t>
+    <t xml:space="preserve"> قصر الثقافة في الشارقة</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-438</t>
@@ -34237,7 +33941,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> فندق روتانا خالدية بالاس فندق روتانا خالد يقلص </t>
+    <t xml:space="preserve"> فندق روتانا خالدية بالاس</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-435</t>
@@ -34324,37 +34028,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> رقم مول الامارات على رقم مول الإمارات</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VA did not recignize the Danat Al Emarat Hospital instead captured as Nanette Al Emarat Hospital.nd for the 2nd time it captured as Danat Al Mada Hospital. Record file is clear from customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: d38a986b8a37_2681dce0-34e9-11e9-8023-f9845d518eae&lt;br&gt;
-Conversation Status: delegated&lt;br&gt;
-EDUID: 5c6d0eff000500000a33a41423330002&lt;br&gt;
-Account Number: 026182698&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;VA did not recignize the Danat Al Emarat Hospital instead captured as Nanette Al Emarat Hospital&lt;br&gt;
-And for the 2nd time it captured as Danat Al Mada Hospital. Record file is clear from customer&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" mat-table="" ng-reflect-data-source="[object Object],[object Object" _ngcontent-c13=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c13=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;Nanette Al Emarat Hospital&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;Okay, so you would like to know the details of Nanette Al Emarat Hospital right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c13=""&gt;0.8346&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c13=""&gt;establishment: Nanette Al Emarat Hospital&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c13=""&gt;20/02/19 12:26:00 pm&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-</t>
+    <t xml:space="preserve"> رقم مول الامارات</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-429</t>
@@ -34414,7 +34088,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> مطعم كيكال مطعم كتكوت </t>
+    <t xml:space="preserve"> مطعم كيكال </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-425</t>
@@ -34822,7 +34496,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> الاجازة السعيدة الرقة الفائدة مطعم </t>
+    <t xml:space="preserve"> الاجازة السعيدة</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-423</t>
@@ -34988,7 +34662,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مجموعة كانو مجموعة كيلوا </t>
+    <t xml:space="preserve"> مجموعة كانو </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-422</t>
@@ -35084,7 +34758,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> اتصالات الغربية إتصالات الغربية</t>
+    <t xml:space="preserve"> اتصالات الغربية</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-420</t>
@@ -35188,7 +34862,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مكافئات مزيد عايز رقم الذيد </t>
+    <t xml:space="preserve"> مكافئات مزيد </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-419</t>
@@ -35275,44 +34949,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مطعم فش اند جبس مطعم أبي مطعم كيش الجبس</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-418</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "HALA PHARMACY", VA recognised as "hello pharmacy/I love pharmacy"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: d38a986b8a37_85c5db90-34f1-11e9-9649-9943c4c18191&lt;br&gt;
-EDUID: 5c6d1d0c000b00000a33a41423330002&lt;br&gt;
-Account Number: 065043238&lt;br&gt;
-&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;customer requested "HALA PHARMACY", VA recognised as "hello pharmacy/I love pharmacy"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c13=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c13="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;hello pharmacy&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Hello! I am your virtual assistant from Etisalat. Could you please specify the name of the place you are looking for?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;ChitChat.GreetHello&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;0.9621&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c13="" mat-cell=""&gt;establishment: pharmacy&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c13="" mat-cell=""&gt;20/02/19 1:25:55 pm&lt;/td&gt;
-		&lt;/tr&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c13="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;I love pharmacy&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Okay, so you would like to know the details of pharmacy right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Confirmation&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;0.93&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c13="" mat-cell=""&gt;establishment: pharmacy&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c13="" mat-cell=""&gt;20/02/19 1:26:08 pm&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-</t>
+    <t xml:space="preserve"> مطعم فش اند جبس</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-413</t>
@@ -35399,7 +35036,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> رقم تسهيل رقم توكيل</t>
+    <t xml:space="preserve"> رقم تسهيل</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-411</t>
@@ -35504,7 +35141,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> بقالة سفاري رقم سفاري بقالت سفاري</t>
+    <t xml:space="preserve"> بقالة سفاري</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-409</t>
@@ -35609,7 +35246,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفى برجيل مستشفى جيل بالشفاء برج جيل</t>
+    <t xml:space="preserve"> مستشفى برجيل</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-408</t>
@@ -35999,7 +35636,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مطعم بحه الزليخه عايز رقم بحرف </t>
+    <t xml:space="preserve"> مطعم بحه</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-407</t>
@@ -36086,9 +35723,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفى برجيل مستشفى بردويل</t>
-  </si>
-  <si>
     <t xml:space="preserve">AVAT-406</t>
   </si>
   <si>
@@ -36210,42 +35844,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفى خليفة عجمان ارسل لي في عجمان مستشفى خليفة عجمان</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "julphar pharmacy", VA recognised as "Khor pharmacy/good for pharmacy"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 1da6036f97c0_27406660-34f3-11e9-b36c-47a9b5a11945&lt;br&gt;
-EDUID: 5c6d1fd5001700000a33a41423330002&lt;br&gt;
-Account Number: 0507507172&lt;/p&gt;
-&lt;p&gt;customer requested "julphar pharmacy", VA recognised as "Khor pharmacy/good for pharmacy"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c13=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c13="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Khor pharmacy&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;Okay, so you would like to know the details of Khor pharmacy right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c13="" mat-cell=""&gt;0.6951&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c13="" mat-cell=""&gt;locality: Khor (Al Khor) establishment: Khor pharmacy&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c13="" mat-cell=""&gt;
-			&lt;p&gt;20/02/19 1:37:36 pm&lt;/p&gt;
-			&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-			&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;div class="cdk-overlay-backdrop cdk-overlay-dark-backdrop cdk-overlay-backdrop-showing"&gt;&amp;nbsp;&lt;/div&gt;
-&lt;div class="cdk-global-overlay-wrapper" style="justify-content: center; align-items: center;" dir="ltr"&gt;&amp;nbsp;&lt;/div&gt;
-</t>
+    <t xml:space="preserve"> مستشفى خليفة عجمان</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-403</t>
@@ -36512,7 +36111,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفي الزليخه لا </t>
+    <t xml:space="preserve"> مستشفي الزليخه </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-399</t>
@@ -36740,7 +36339,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> مستشفي الجرهود ممكن </t>
+    <t xml:space="preserve"> مستشفي الجرهود</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-397</t>
@@ -36864,7 +36463,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> اريد رقم ماكدونالد اريد رقم مكتوم اريد رقم مكتوم ال</t>
+    <t xml:space="preserve"> اريد رقم ماكدونالد</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-393</t>
@@ -36988,7 +36587,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> أريد رقم اكسنت تول اريد رقم إكس الندود غنتوت</t>
+    <t xml:space="preserve"> أريد رقم اكسنت تول</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-391</t>
@@ -37175,7 +36774,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كنتاكي العقه </t>
+    <t xml:space="preserve"> كنتاكي  </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-388</t>
@@ -37628,7 +37227,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> المسيله المثل </t>
+    <t xml:space="preserve"> المسيله  </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-386</t>
@@ -38016,7 +37615,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> المعز للمقاولا شركة الموعد أبوظبي </t>
+    <t xml:space="preserve"> المعز للمقاولات</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-382</t>
@@ -38433,7 +38032,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> ستار باكس عايز رقم قلبك </t>
+    <t xml:space="preserve"> ستار باكس</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-373</t>
@@ -38557,7 +38156,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> شركة الاردن وأبو ظبي للتخليص والشحن البري شركة الاردن وأبو طبري للتخليص والشحن البردي شركة الاردن وا أبوظبي للتخليص والشحن البري</t>
+    <t xml:space="preserve"> شركة الاردن وأبو ظبي للتخليص والشحن البري</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-372</t>
@@ -38890,7 +38489,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> بدي رقم حسن ابحث عن جزيرة سناب</t>
+    <t xml:space="preserve"> بدي رقم حسن</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-366</t>
@@ -39069,7 +38668,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> خمسه مصفح </t>
+    <t xml:space="preserve"> خمسه  </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-363</t>
@@ -39193,7 +38792,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> رقم المزبله رقم المقبل الجزيرة</t>
+    <t xml:space="preserve"> رقم المزبله</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-361</t>
@@ -39417,9 +39016,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كنتاكي يس </t>
-  </si>
-  <si>
     <t xml:space="preserve">AVAT-359</t>
   </si>
   <si>
@@ -39519,9 +39115,6 @@
 ACCOUNT NUMBER : 0504064378
 </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> كنتاكي القير </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-357</t>
@@ -39686,9 +39279,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كنتاكي ممكن تيجي </t>
-  </si>
-  <si>
     <t xml:space="preserve">AVAT-356</t>
   </si>
   <si>
@@ -39829,7 +39419,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> سن اند ساند سبورتس الميدان سن اند ساند سبورتس </t>
+    <t xml:space="preserve"> سن اند ساند سبورتس</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-354</t>
@@ -39989,9 +39579,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كنتاكي أي</t>
-  </si>
-  <si>
     <t xml:space="preserve">AVAT-353</t>
   </si>
   <si>
@@ -40132,7 +39719,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> صن اند ساند سبورتس البستان صن اند ساند </t>
+    <t xml:space="preserve"> صن اند ساند سبورتس</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-352</t>
@@ -40219,7 +39806,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> سنو وايت وايت</t>
+    <t xml:space="preserve"> سنو وايت </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-351</t>
@@ -40343,7 +39930,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> سنو وايت واي رقم واي </t>
+    <t xml:space="preserve"> سنو وايت</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-349</t>
@@ -40497,7 +40084,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> أنا عاوز رقم اتصالات أنا عاوز رقم غلط </t>
+    <t xml:space="preserve"> أنا عاوز رقم اتصالات</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-346</t>
@@ -40643,7 +40230,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> سوان لصناعة مفاتيح التحكم الكهربانيه الصوان لصناعة مفاتيح التحكيم الكهربانية</t>
+    <t xml:space="preserve"> سوان لصناعة مفاتيح التحكم الكهربانيه </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-341</t>
@@ -40738,9 +40325,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> كنتاكي دقيقه</t>
-  </si>
-  <si>
     <t xml:space="preserve">AVAT-340</t>
   </si>
   <si>
@@ -40825,7 +40409,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> من فضلك رقم اتصالات رقم بكثرة</t>
+    <t xml:space="preserve"> من فضلك رقم اتصالات</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-339</t>
@@ -40906,9 +40490,6 @@
       <t xml:space="preserve">ممكن دقيقة
 </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> كنتاكي ممكن دقيقة</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-328</t>
@@ -41003,7 +40584,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> عيسي لتاجير السيارات ايش أكتيف الفجيرة</t>
+    <t xml:space="preserve"> عيسي لتاجير السيارات</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-321</t>
@@ -41176,7 +40757,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> الأسوار لقطع غيار السيارات الأسوأ لقطع غيار السيارات </t>
+    <t xml:space="preserve"> الأسوار لقطع غيار السيارات</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-314</t>
@@ -41331,73 +40912,6 @@
     <t xml:space="preserve">أس تي أم ميدل ايست </t>
   </si>
   <si>
-    <t xml:space="preserve">AVAT-308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "Paris gallery", VA recognised as "no I said security/Baniyas"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;br&gt;
-Conversation ID: 5386f0c36e0d_2eb60bc0-3502-11e9-963b-758e7e407292&lt;br&gt;
-EDUID: 5c6d390c002d00000a33a41423330002&lt;br&gt;
-Account Number: 0568630826&lt;/p&gt;
-&lt;p&gt;customer requested "Paris gallery", VA recognised as "no I said security/Baniyas"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c21=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Baniyas&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Okay, so you would like to know the details of Baniyas right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;None&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;1&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;establishment: Baniyas locality: Baniyas&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;20/02/19 3:25:11 pm&lt;/td&gt;
-		&lt;/tr&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;no I said security&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Okay, so you would like to know the details of Baniyas right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;AgentHandover&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;0.5987&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;&amp;nbsp;&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;20/02/19 3:25:24 pm&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "Carefour", VA recognised as "Gurfa/telephone"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 1da6036f97c0_1ab5de70-3516-11e9-8023-f9845d518eae&lt;br&gt;
-EDUID: 5c6d5a78001800000a33a41423330002&lt;br&gt;
-Account Number: 0507285668&lt;/p&gt;
-&lt;p&gt;customer requested "Carefour", VA recognised as "Gurfa/telephone"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c21=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Gurfa&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Okay, so you would like to know the details of Gurfa right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;None&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;1&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;establishment: Gurfa locality: Gurfa&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;20/02/19 5:47:47 pm&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">AVAT-288</t>
   </si>
   <si>
@@ -41549,7 +41063,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ايوا ليوا</t>
+    <t xml:space="preserve">ايوا </t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-286</t>
@@ -41576,114 +41090,6 @@
   </si>
   <si>
     <t xml:space="preserve">أي منطقة </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-279</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "Dubai police", VA recognised as "Dubai Polysys/ Dubai"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: d38a986b8a37_9227a480-3b1e-11e9-b36c-47a9b5a11945&lt;br&gt;
-EDUID: 5c7779a2000100000a33a41423330002&lt;br&gt;
-Account Number: 888888888888&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;customer requested "Dubai police", VA recognised as "Dubai Polysys/ Dubai&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c21=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Dubai&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;I didn't get that. Could you please specify the name of the place you are looking for?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;0.9951&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;emirate: Dubai&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;28/02/19 10:03:33 am&lt;/td&gt;
-		&lt;/tr&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Dubai Polysys&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Okay, so you would like to know the details of Dubai Polysys right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;0.9952&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;emirate: Dubai establishment: Dubai Polysys&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;28/02/19 10:03:39 am&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-277</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "technology source", VA recognised as "corniche/technology Park"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 5386f0c36e0d_2236cdc0-3b20-11e9-9649-9943c4c18191&lt;br&gt;
-EDUID: 5c777c47000900000a33a41423330002&lt;br&gt;
-Account Number: 0564841599&lt;/p&gt;
-&lt;p&gt;customer requested "technology source", VA recognised as "corniche/technology Park"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c21=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;corniche&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;I didn't get that. Could you please specify the name of the place you are looking for?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;None&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;1&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;locality: corniche (Corniche)&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;28/02/19 10:14:42 am&lt;/td&gt;
-		&lt;/tr&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;technology Park&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Hello! I am your virtual assistant from Etisalat. I didn't get that. Could you please specify the name of the place you are looking for?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;ChitChat.GreetHello&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;0.7749&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;establishment: technology Park locality: technology Park (Technology Park)&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;
-			&lt;p&gt;28/02/19 10:14:53 am&lt;/p&gt;
-			&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-			&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested "Mall of emirates ", Entity recognised as "Margham//Monicals the emirates"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: da7df33d332a_4cb12c70-3b21-11e9-963b-758e7e407292&lt;br&gt;
-EDUID: 5c777e3c001000000a33a41423330002&lt;br&gt;
-Account Number: 0506764660&lt;/p&gt;
-&lt;p&gt;customer requested "Mall of emirates ", Entity recognised as "Margham//Monicals the emirates"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c21=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" mat-row="" _ngcontent-c21=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Margham&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;Okay, so you would like to know the details of Margham right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;None&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" mat-cell="" _ngcontent-c21=""&gt;1&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" mat-cell="" _ngcontent-c21=""&gt;establishment: Margham locality: Margham&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" mat-cell="" _ngcontent-c21=""&gt;
-			&lt;p&gt;28/02/19 10:23:02 am&lt;/p&gt;
-			&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-			&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-			&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-267</t>
@@ -41774,63 +41180,6 @@
   </si>
   <si>
     <t xml:space="preserve"> حلويات فراس</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested Al Baba Al Mumtaza Sweets, VA recognised as "Lehbab Mumtaza sweets/ Abbaba Mumtaza sweets"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversation ID: d38a986b8a37_d7ac3c20-3522-11e9-963b-758e7e407292
-EDUID: 5c6d6fcb000200000a33a41423330002
-Account Number: 0564275237
-customer requested Al Baba Al Mumtaza Sweets, VA recognised as "Lehbab Mumtaza sweets/ Abbaba Mumtaza sweets"
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested A A SONS , VA recognised as "and Sons/ any sun"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Conversation ID: 1da6036f97c0_40c8e960-352d-11e9-b36c-47a9b5a11945&lt;br&gt;
-EDUID: 5c6d814f000200000a33a41423330002&lt;br&gt;
-Account Number:0507285668&lt;/p&gt;
-&lt;p&gt;customer requested A A SONS , VA recognised as "and Sons/ any sun"&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table class="flex-container-card mat-table" role="grid" style="border-collapse: collapse;" ng-reflect-data-source="[object Object],[object Object" mat-table="" _ngcontent-c21=""&gt;
-	&lt;tbody&gt;
-		&lt;tr class="mat-row ng-star-inserted" role="row" _ngcontent-c21="" mat-row=""&gt;
-			&lt;td class="mat-cell cdk-column-user mat-column-user ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;and Sons&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-virtualAgent mat-column-virtualAgent ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;Okay, so you would like to know the details of and Sons right?&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-callReason mat-column-callReason ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;establishment_inquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-intent mat-column-intent ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;EstablishmentDetailsInquiry&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-score mat-column-score ng-star-inserted" role="gridcell" _ngcontent-c21="" mat-cell=""&gt;0.4577&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-entities mat-column-entities ng-star-inserted" role="gridcell" style="white-space: pre-line;" _ngcontent-c21="" mat-cell=""&gt;establishment: and Sons&lt;/td&gt;
-			&lt;td class="mat-cell cdk-column-datetime mat-column-datetime ng-star-inserted" role="gridcell" nowrap="nowrap" _ngcontent-c21="" mat-cell=""&gt;
-			&lt;p&gt;20/02/19 8:33:30 pm&lt;/p&gt;
-			&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-			&lt;/td&gt;
-		&lt;/tr&gt;
-	&lt;/tbody&gt;
-&lt;/table&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVAT-249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer requested Ewan Ajman Suites Hotel, VA captured Establishment as Ajman Port/Ajman insurance Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversation ID: 5386f0c36e0d_503b7fd0-353b-11e9-8023-f9845d518eae
-EDUID: 5c6d98db001200000a33a41423330002
-Account Number: 067141721
-customer requested Ewan Ajman Suites Hotel, VA captured Establishment as Ajman Port/Ajman insurance Company
-</t>
   </si>
   <si>
     <t xml:space="preserve">AVAT-213</t>
@@ -42232,10 +41581,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G325"/>
+  <dimension ref="A1:G306"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D212" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E212" activeCellId="0" sqref="E212"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42244,7 +41593,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="212.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="48.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -45977,6 +45326,9 @@
       <c r="E219" s="2" t="s">
         <v>861</v>
       </c>
+      <c r="F219" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="220" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
@@ -46029,12 +45381,12 @@
         <v>873</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="415.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
         <v>874</v>
       </c>
       <c r="B223" s="0" t="n">
-        <v>94951</v>
+        <v>94945</v>
       </c>
       <c r="C223" s="0" t="s">
         <v>875</v>
@@ -46042,16 +45394,16 @@
       <c r="D223" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="E223" s="0" t="s">
+      <c r="E223" s="2" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="251.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
         <v>878</v>
       </c>
       <c r="B224" s="0" t="n">
-        <v>94945</v>
+        <v>94943</v>
       </c>
       <c r="C224" s="0" t="s">
         <v>879</v>
@@ -46063,12 +45415,12 @@
         <v>881</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="251.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="357.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
         <v>882</v>
       </c>
       <c r="B225" s="0" t="n">
-        <v>94943</v>
+        <v>94940</v>
       </c>
       <c r="C225" s="0" t="s">
         <v>883</v>
@@ -46080,12 +45432,12 @@
         <v>885</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="357.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
         <v>886</v>
       </c>
       <c r="B226" s="0" t="n">
-        <v>94940</v>
+        <v>94920</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>887</v>
@@ -46102,7 +45454,7 @@
         <v>890</v>
       </c>
       <c r="B227" s="0" t="n">
-        <v>94920</v>
+        <v>94918</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>891</v>
@@ -46119,7 +45471,7 @@
         <v>894</v>
       </c>
       <c r="B228" s="0" t="n">
-        <v>94918</v>
+        <v>94917</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>895</v>
@@ -46131,12 +45483,12 @@
         <v>897</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
         <v>898</v>
       </c>
       <c r="B229" s="0" t="n">
-        <v>94917</v>
+        <v>94916</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>899</v>
@@ -46148,12 +45500,12 @@
         <v>901</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
         <v>902</v>
       </c>
       <c r="B230" s="0" t="n">
-        <v>94916</v>
+        <v>94915</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>903</v>
@@ -46170,7 +45522,7 @@
         <v>906</v>
       </c>
       <c r="B231" s="0" t="n">
-        <v>94915</v>
+        <v>94912</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>907</v>
@@ -46187,7 +45539,7 @@
         <v>910</v>
       </c>
       <c r="B232" s="0" t="n">
-        <v>94912</v>
+        <v>94911</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>911</v>
@@ -46199,12 +45551,12 @@
         <v>913</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
         <v>914</v>
       </c>
       <c r="B233" s="0" t="n">
-        <v>94911</v>
+        <v>94910</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>915</v>
@@ -46216,12 +45568,12 @@
         <v>917</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
         <v>918</v>
       </c>
       <c r="B234" s="0" t="n">
-        <v>94910</v>
+        <v>94909</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>919</v>
@@ -46238,7 +45590,7 @@
         <v>922</v>
       </c>
       <c r="B235" s="0" t="n">
-        <v>94909</v>
+        <v>94907</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>923</v>
@@ -46250,12 +45602,12 @@
         <v>925</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
         <v>926</v>
       </c>
       <c r="B236" s="0" t="n">
-        <v>94907</v>
+        <v>94906</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>927</v>
@@ -46267,12 +45619,12 @@
         <v>929</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
         <v>930</v>
       </c>
       <c r="B237" s="0" t="n">
-        <v>94906</v>
+        <v>94905</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>931</v>
@@ -46284,12 +45636,12 @@
         <v>933</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
         <v>934</v>
       </c>
       <c r="B238" s="0" t="n">
-        <v>94905</v>
+        <v>94901</v>
       </c>
       <c r="C238" s="0" t="s">
         <v>935</v>
@@ -46298,219 +45650,219 @@
         <v>936</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
+        <v>937</v>
+      </c>
+      <c r="B239" s="0" t="n">
+        <v>94899</v>
+      </c>
+      <c r="C239" s="0" t="s">
         <v>938</v>
       </c>
-      <c r="B239" s="0" t="n">
-        <v>94901</v>
-      </c>
-      <c r="C239" s="0" t="s">
+      <c r="D239" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="D239" s="1" t="s">
+      <c r="E239" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="E239" s="2" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
+        <v>941</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>94895</v>
+      </c>
+      <c r="C240" s="0" t="s">
         <v>942</v>
       </c>
-      <c r="B240" s="0" t="n">
-        <v>94899</v>
-      </c>
-      <c r="C240" s="0" t="s">
+      <c r="D240" s="1" t="s">
         <v>943</v>
       </c>
-      <c r="D240" s="1" t="s">
+      <c r="E240" s="2" t="s">
         <v>944</v>
-      </c>
-      <c r="E240" s="2" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="B241" s="0" t="n">
+        <v>94888</v>
+      </c>
+      <c r="C241" s="0" t="s">
         <v>946</v>
       </c>
-      <c r="B241" s="0" t="n">
-        <v>94895</v>
-      </c>
-      <c r="C241" s="0" t="s">
+      <c r="D241" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="D241" s="1" t="s">
+      <c r="E241" s="2" t="s">
         <v>948</v>
       </c>
-      <c r="E241" s="2" t="s">
+    </row>
+    <row r="242" customFormat="false" ht="800" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
         <v>949</v>
       </c>
+      <c r="B242" s="0" t="n">
+        <v>94885</v>
+      </c>
+      <c r="C242" s="0" t="s">
+        <v>950</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="E242" s="0" t="s">
+        <v>952</v>
+      </c>
     </row>
-    <row r="242" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="0" t="s">
-        <v>950</v>
-      </c>
-      <c r="B242" s="0" t="n">
-        <v>94888</v>
-      </c>
-      <c r="C242" s="0" t="s">
-        <v>951</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>952</v>
-      </c>
-      <c r="E242" s="2" t="s">
+    <row r="243" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
         <v>953</v>
       </c>
+      <c r="B243" s="0" t="n">
+        <v>94881</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>956</v>
+      </c>
     </row>
-    <row r="243" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="0" t="s">
-        <v>954</v>
-      </c>
-      <c r="B243" s="0" t="n">
-        <v>94885</v>
-      </c>
-      <c r="C243" s="0" t="s">
-        <v>955</v>
-      </c>
-      <c r="D243" s="1" t="s">
-        <v>956</v>
-      </c>
-      <c r="E243" s="0" t="s">
+    <row r="244" customFormat="false" ht="115.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
         <v>957</v>
       </c>
+      <c r="B244" s="0" t="n">
+        <v>94878</v>
+      </c>
+      <c r="C244" s="0" t="s">
+        <v>958</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>960</v>
+      </c>
     </row>
-    <row r="244" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="0" t="s">
-        <v>958</v>
-      </c>
-      <c r="B244" s="0" t="n">
-        <v>94881</v>
-      </c>
-      <c r="C244" s="0" t="s">
-        <v>959</v>
-      </c>
-      <c r="D244" s="1" t="s">
-        <v>960</v>
-      </c>
-      <c r="E244" s="2" t="s">
+    <row r="245" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="245" customFormat="false" ht="115.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="0" t="s">
+      <c r="B245" s="0" t="n">
+        <v>94876</v>
+      </c>
+      <c r="C245" s="0" t="s">
         <v>962</v>
       </c>
-      <c r="B245" s="0" t="n">
-        <v>94878</v>
-      </c>
-      <c r="C245" s="0" t="s">
+      <c r="D245" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="D245" s="1" t="s">
+      <c r="E245" s="2" t="s">
         <v>964</v>
-      </c>
-      <c r="E245" s="2" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
+        <v>965</v>
+      </c>
+      <c r="B246" s="0" t="n">
+        <v>94874</v>
+      </c>
+      <c r="C246" s="0" t="s">
         <v>966</v>
       </c>
-      <c r="B246" s="0" t="n">
-        <v>94876</v>
-      </c>
-      <c r="C246" s="0" t="s">
+      <c r="D246" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="E246" s="2" t="s">
         <v>968</v>
       </c>
-      <c r="E246" s="2" t="s">
+    </row>
+    <row r="247" customFormat="false" ht="346.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
         <v>969</v>
       </c>
+      <c r="B247" s="0" t="n">
+        <v>94871</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>970</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>972</v>
+      </c>
     </row>
-    <row r="247" customFormat="false" ht="349.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="0" t="s">
-        <v>970</v>
-      </c>
-      <c r="B247" s="0" t="n">
-        <v>94874</v>
-      </c>
-      <c r="C247" s="0" t="s">
-        <v>971</v>
-      </c>
-      <c r="D247" s="1" t="s">
-        <v>972</v>
-      </c>
-      <c r="E247" s="2" t="s">
+    <row r="248" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
         <v>973</v>
       </c>
+      <c r="B248" s="0" t="n">
+        <v>94857</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>974</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>976</v>
+      </c>
     </row>
-    <row r="248" customFormat="false" ht="346.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="0" t="s">
-        <v>974</v>
-      </c>
-      <c r="B248" s="0" t="n">
-        <v>94871</v>
-      </c>
-      <c r="C248" s="0" t="s">
-        <v>975</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>976</v>
-      </c>
-      <c r="E248" s="2" t="s">
+    <row r="249" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
         <v>977</v>
       </c>
+      <c r="B249" s="0" t="n">
+        <v>94574</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>980</v>
+      </c>
     </row>
-    <row r="249" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="0" t="s">
-        <v>978</v>
-      </c>
-      <c r="B249" s="0" t="n">
-        <v>94857</v>
-      </c>
-      <c r="C249" s="0" t="s">
-        <v>979</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>980</v>
-      </c>
-      <c r="E249" s="2" t="s">
+    <row r="250" customFormat="false" ht="101.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
         <v>981</v>
       </c>
+      <c r="B250" s="0" t="n">
+        <v>94581</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>984</v>
+      </c>
     </row>
-    <row r="250" customFormat="false" ht="241" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="0" t="s">
-        <v>982</v>
-      </c>
-      <c r="B250" s="0" t="n">
-        <v>94837</v>
-      </c>
-      <c r="C250" s="0" t="s">
-        <v>983</v>
-      </c>
-      <c r="D250" s="1" t="s">
-        <v>984</v>
-      </c>
-      <c r="E250" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="132.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="591" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
         <v>985</v>
       </c>
       <c r="B251" s="0" t="n">
-        <v>94442</v>
+        <v>94655</v>
       </c>
       <c r="C251" s="0" t="s">
         <v>986</v>
@@ -46518,798 +45870,801 @@
       <c r="D251" s="1" t="s">
         <v>987</v>
       </c>
-      <c r="E251" s="0" t="n">
-        <v>2</v>
+      <c r="E251" s="2" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B252" s="0" t="n">
-        <v>94574</v>
+        <v>94771</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="101.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B253" s="0" t="n">
-        <v>94581</v>
+        <v>94767</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="591" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B254" s="0" t="n">
-        <v>94655</v>
+        <v>94761</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E254" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="262.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B255" s="0" t="n">
-        <v>94812</v>
+        <v>94742</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E255" s="0" t="s">
-        <v>877</v>
+        <v>1003</v>
+      </c>
+      <c r="E255" s="2" t="s">
+        <v>1004</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="623.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B256" s="0" t="n">
-        <v>94771</v>
+        <v>94740</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E256" s="2" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="101.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="126.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B257" s="0" t="n">
-        <v>94767</v>
+        <v>94737</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="164.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B258" s="0" t="n">
-        <v>94761</v>
+        <v>94729</v>
       </c>
       <c r="C258" s="0" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="273.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="675" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B259" s="0" t="n">
-        <v>94756</v>
+        <v>94723</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>1017</v>
-      </c>
-      <c r="E259" s="0" t="n">
-        <v>2</v>
+        <v>1019</v>
+      </c>
+      <c r="E259" s="2" t="s">
+        <v>1020</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="101.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="379.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="B260" s="0" t="n">
-        <v>94753</v>
+        <v>94721</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>1020</v>
+        <v>1023</v>
       </c>
       <c r="E260" s="2" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="306.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="B261" s="0" t="n">
-        <v>94748</v>
+        <v>94720</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="E261" s="0" t="s">
-        <v>877</v>
+        <v>1027</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>1028</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="350" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c r="B262" s="0" t="n">
-        <v>94743</v>
+        <v>94718</v>
       </c>
       <c r="C262" s="0" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>1027</v>
-      </c>
-      <c r="E262" s="0" t="s">
-        <v>1028</v>
+        <v>1031</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>1032</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="126.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="B263" s="0" t="n">
-        <v>94742</v>
+        <v>94717</v>
       </c>
       <c r="C263" s="0" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>1032</v>
+        <v>1036</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="623.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>1033</v>
+        <v>1037</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>94740</v>
+        <v>94710</v>
       </c>
       <c r="C264" s="0" t="s">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>1035</v>
+        <v>1039</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>1036</v>
+        <v>1040</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="126.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="B265" s="0" t="n">
-        <v>94737</v>
+        <v>94707</v>
       </c>
       <c r="C265" s="0" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="284.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="B266" s="0" t="n">
-        <v>94733</v>
+        <v>94705</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>1043</v>
-      </c>
-      <c r="E266" s="0" t="n">
-        <v>2</v>
+        <v>1047</v>
+      </c>
+      <c r="E266" s="2" t="s">
+        <v>1048</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="164.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="685.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>1044</v>
+        <v>1049</v>
       </c>
       <c r="B267" s="0" t="n">
-        <v>94729</v>
+        <v>94704</v>
       </c>
       <c r="C267" s="0" t="s">
-        <v>1045</v>
+        <v>1050</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>1046</v>
+        <v>1051</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>1047</v>
+        <v>1052</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="675" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>94703</v>
+      </c>
+      <c r="C268" s="0" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E268" s="2" t="s">
         <v>1048</v>
       </c>
-      <c r="B268" s="0" t="n">
-        <v>94723</v>
-      </c>
-      <c r="C268" s="0" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D268" s="1" t="s">
-        <v>1050</v>
-      </c>
-      <c r="E268" s="2" t="s">
-        <v>1051</v>
-      </c>
     </row>
-    <row r="269" customFormat="false" ht="379.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>1052</v>
+        <v>1056</v>
       </c>
       <c r="B269" s="0" t="n">
-        <v>94721</v>
+        <v>94702</v>
       </c>
       <c r="C269" s="0" t="s">
-        <v>1053</v>
+        <v>1057</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>1054</v>
+        <v>1058</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="550.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>94720</v>
+        <v>94698</v>
       </c>
       <c r="C270" s="0" t="s">
-        <v>1057</v>
+        <v>1061</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>1059</v>
+        <v>1063</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="463.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>1060</v>
+        <v>1064</v>
       </c>
       <c r="B271" s="0" t="n">
-        <v>94718</v>
+        <v>94692</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>1061</v>
+        <v>1065</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>1062</v>
+        <v>1066</v>
       </c>
       <c r="E271" s="2" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="126.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="139.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="B272" s="0" t="n">
-        <v>94717</v>
+        <v>94689</v>
       </c>
       <c r="C272" s="0" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="E272" s="2" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="350" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>1068</v>
+        <v>1072</v>
       </c>
       <c r="B273" s="0" t="n">
-        <v>94715</v>
+        <v>94681</v>
       </c>
       <c r="C273" s="0" t="s">
-        <v>1069</v>
+        <v>1073</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>1070</v>
-      </c>
-      <c r="E273" s="0" t="s">
-        <v>877</v>
+        <v>1074</v>
+      </c>
+      <c r="E273" s="2" t="s">
+        <v>1075</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="436.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>1071</v>
+        <v>1076</v>
       </c>
       <c r="B274" s="0" t="n">
-        <v>94710</v>
+        <v>94679</v>
       </c>
       <c r="C274" s="0" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>1073</v>
+        <v>1078</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>1074</v>
+        <v>1079</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="789.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>1075</v>
+        <v>1080</v>
       </c>
       <c r="B275" s="0" t="n">
-        <v>94707</v>
+        <v>94672</v>
       </c>
       <c r="C275" s="0" t="s">
-        <v>1076</v>
+        <v>1081</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>1077</v>
+        <v>1082</v>
       </c>
       <c r="E275" s="2" t="s">
-        <v>1078</v>
+        <v>1083</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="923.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>94668</v>
+      </c>
+      <c r="C276" s="0" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E276" s="2" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="789.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>94663</v>
+      </c>
+      <c r="C277" s="0" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E277" s="2" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="139.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B278" s="0" t="n">
+        <v>94645</v>
+      </c>
+      <c r="C278" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="504.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>94643</v>
+      </c>
+      <c r="C279" s="0" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E279" s="2" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="96.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>94638</v>
+      </c>
+      <c r="C280" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="379.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B281" s="0" t="n">
+        <v>94637</v>
+      </c>
+      <c r="C281" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E281" s="2" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B282" s="0" t="n">
+        <v>94634</v>
+      </c>
+      <c r="C282" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E282" s="2" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="493.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B283" s="0" t="n">
+        <v>94632</v>
+      </c>
+      <c r="C283" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E283" s="2" t="s">
         <v>1079</v>
       </c>
-      <c r="B276" s="0" t="n">
-        <v>94705</v>
-      </c>
-      <c r="C276" s="0" t="s">
-        <v>1080</v>
-      </c>
-      <c r="D276" s="1" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E276" s="2" t="s">
-        <v>1082</v>
-      </c>
     </row>
-    <row r="277" customFormat="false" ht="685.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="0" t="s">
-        <v>1083</v>
-      </c>
-      <c r="B277" s="0" t="n">
-        <v>94704</v>
-      </c>
-      <c r="C277" s="0" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D277" s="1" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E277" s="2" t="s">
-        <v>1086</v>
+    <row r="284" customFormat="false" ht="80.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B284" s="0" t="n">
+        <v>94630</v>
+      </c>
+      <c r="C284" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F284" s="0" t="s">
+        <v>527</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="0" t="s">
-        <v>1087</v>
-      </c>
-      <c r="B278" s="0" t="n">
-        <v>94703</v>
-      </c>
-      <c r="C278" s="0" t="s">
-        <v>1088</v>
-      </c>
-      <c r="D278" s="1" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E278" s="2" t="s">
-        <v>1090</v>
+    <row r="285" customFormat="false" ht="357.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>94628</v>
+      </c>
+      <c r="C285" s="0" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E285" s="2" t="s">
+        <v>849</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="0" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B279" s="0" t="n">
-        <v>94702</v>
-      </c>
-      <c r="C279" s="0" t="s">
-        <v>1092</v>
-      </c>
-      <c r="D279" s="1" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E279" s="2" t="s">
-        <v>1094</v>
+    <row r="286" customFormat="false" ht="128.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>94626</v>
+      </c>
+      <c r="C286" s="0" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E286" s="2" t="s">
+        <v>1123</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="393.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="0" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B280" s="0" t="n">
-        <v>94697</v>
-      </c>
-      <c r="C280" s="0" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D280" s="1" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E280" s="0" t="s">
-        <v>877</v>
+    <row r="287" customFormat="false" ht="455.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>94623</v>
+      </c>
+      <c r="C287" s="0" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E287" s="2" t="s">
+        <v>933</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="550.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="0" t="s">
-        <v>1098</v>
-      </c>
-      <c r="B281" s="0" t="n">
-        <v>94698</v>
-      </c>
-      <c r="C281" s="0" t="s">
-        <v>1099</v>
-      </c>
-      <c r="D281" s="1" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E281" s="2" t="s">
-        <v>1101</v>
+    <row r="288" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>94622</v>
+      </c>
+      <c r="C288" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E288" s="2" t="s">
+        <v>1130</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="463.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="0" t="s">
-        <v>1102</v>
-      </c>
-      <c r="B282" s="0" t="n">
-        <v>94692</v>
-      </c>
-      <c r="C282" s="0" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D282" s="1" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E282" s="2" t="s">
-        <v>1105</v>
+    <row r="289" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B289" s="0" t="n">
+        <v>94615</v>
+      </c>
+      <c r="C289" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E289" s="2" t="s">
+        <v>1134</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="139.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="0" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B283" s="0" t="n">
-        <v>94689</v>
-      </c>
-      <c r="C283" s="0" t="s">
-        <v>1107</v>
-      </c>
-      <c r="D283" s="1" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E283" s="2" t="s">
-        <v>1109</v>
+    <row r="290" customFormat="false" ht="93.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B290" s="0" t="n">
+        <v>94612</v>
+      </c>
+      <c r="C290" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E290" s="2" t="s">
+        <v>1138</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="0" t="s">
-        <v>1110</v>
-      </c>
-      <c r="B284" s="0" t="n">
-        <v>94681</v>
-      </c>
-      <c r="C284" s="0" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D284" s="1" t="s">
-        <v>1112</v>
-      </c>
-      <c r="E284" s="2" t="s">
-        <v>1113</v>
+    <row r="291" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B291" s="0" t="n">
+        <v>94607</v>
+      </c>
+      <c r="C291" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E291" s="2" t="s">
+        <v>1142</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="436.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="0" t="s">
-        <v>1114</v>
-      </c>
-      <c r="B285" s="0" t="n">
-        <v>94679</v>
-      </c>
-      <c r="C285" s="0" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D285" s="1" t="s">
-        <v>1116</v>
-      </c>
-      <c r="E285" s="2" t="s">
-        <v>1117</v>
+    <row r="292" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B292" s="0" t="n">
+        <v>94600</v>
+      </c>
+      <c r="C292" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E292" s="2" t="s">
+        <v>1146</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="789.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="0" t="s">
-        <v>1118</v>
-      </c>
-      <c r="B286" s="0" t="n">
-        <v>94672</v>
-      </c>
-      <c r="C286" s="0" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D286" s="1" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E286" s="2" t="s">
-        <v>1121</v>
+    <row r="293" customFormat="false" ht="44.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>94596</v>
+      </c>
+      <c r="C293" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E293" s="2" t="s">
+        <v>1150</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="923.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="0" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B287" s="0" t="n">
-        <v>94668</v>
-      </c>
-      <c r="C287" s="0" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D287" s="1" t="s">
-        <v>1124</v>
-      </c>
-      <c r="E287" s="2" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="789.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="0" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B288" s="0" t="n">
-        <v>94663</v>
-      </c>
-      <c r="C288" s="0" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D288" s="1" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E288" s="2" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="139.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="0" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B289" s="0" t="n">
-        <v>94645</v>
-      </c>
-      <c r="C289" s="0" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D289" s="1" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E289" s="2" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="504.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="0" t="s">
-        <v>1134</v>
-      </c>
-      <c r="B290" s="0" t="n">
-        <v>94643</v>
-      </c>
-      <c r="C290" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D290" s="1" t="s">
-        <v>1136</v>
-      </c>
-      <c r="E290" s="2" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="96.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="0" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B291" s="0" t="n">
-        <v>94638</v>
-      </c>
-      <c r="C291" s="0" t="s">
-        <v>1138</v>
-      </c>
-      <c r="D291" s="1" t="s">
-        <v>1139</v>
-      </c>
-      <c r="E291" s="2" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="379.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="0" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B292" s="0" t="n">
-        <v>94637</v>
-      </c>
-      <c r="C292" s="0" t="s">
-        <v>1142</v>
-      </c>
-      <c r="D292" s="1" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E292" s="2" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="293" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="0" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B293" s="0" t="n">
-        <v>94634</v>
-      </c>
-      <c r="C293" s="0" t="s">
-        <v>1146</v>
-      </c>
-      <c r="D293" s="1" t="s">
-        <v>1147</v>
-      </c>
-      <c r="E293" s="2" t="s">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="294" customFormat="false" ht="493.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="B294" s="0" t="n">
-        <v>94632</v>
+        <v>94594</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="E294" s="2" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="80.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="B295" s="0" t="n">
-        <v>94630</v>
+        <v>94589</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="E295" s="2" t="s">
-        <v>1156</v>
+        <v>849</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="357.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="93.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B296" s="0" t="n">
-        <v>94628</v>
+        <v>94587</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="E296" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="128.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B297" s="0" t="n">
-        <v>94626</v>
+        <v>94585</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="E297" s="2" t="s">
-        <v>1164</v>
+        <v>933</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="455.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="101.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
         <v>1165</v>
       </c>
       <c r="B298" s="0" t="n">
-        <v>94623</v>
+        <v>94559</v>
       </c>
       <c r="C298" s="0" t="s">
         <v>1166</v>
@@ -47321,12 +46676,12 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="115.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
         <v>1169</v>
       </c>
       <c r="B299" s="0" t="n">
-        <v>94622</v>
+        <v>94547</v>
       </c>
       <c r="C299" s="0" t="s">
         <v>1170</v>
@@ -47338,12 +46693,12 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="82.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
         <v>1173</v>
       </c>
       <c r="B300" s="0" t="n">
-        <v>94615</v>
+        <v>94540</v>
       </c>
       <c r="C300" s="0" t="s">
         <v>1174</v>
@@ -47355,14 +46710,14 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="93.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="330.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
         <v>1177</v>
       </c>
       <c r="B301" s="0" t="n">
-        <v>94612</v>
-      </c>
-      <c r="C301" s="0" t="s">
+        <v>94533</v>
+      </c>
+      <c r="C301" s="2" t="s">
         <v>1178</v>
       </c>
       <c r="D301" s="1" t="s">
@@ -47372,14 +46727,14 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="273.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
         <v>1181</v>
       </c>
       <c r="B302" s="0" t="n">
-        <v>94607</v>
-      </c>
-      <c r="C302" s="0" t="s">
+        <v>94382</v>
+      </c>
+      <c r="C302" s="2" t="s">
         <v>1182</v>
       </c>
       <c r="D302" s="1" t="s">
@@ -47389,392 +46744,69 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
         <v>1185</v>
       </c>
       <c r="B303" s="0" t="n">
-        <v>94600</v>
-      </c>
-      <c r="C303" s="0" t="s">
+        <v>94344</v>
+      </c>
+      <c r="C303" s="2" t="s">
         <v>1186</v>
       </c>
-      <c r="D303" s="1" t="s">
+      <c r="E303" s="2" t="s">
         <v>1187</v>
       </c>
-      <c r="E303" s="2" t="s">
+    </row>
+    <row r="304" customFormat="false" ht="246.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
         <v>1188</v>
       </c>
+      <c r="B304" s="0" t="n">
+        <v>94267</v>
+      </c>
+      <c r="C304" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E304" s="2" t="s">
+        <v>1191</v>
+      </c>
     </row>
-    <row r="304" customFormat="false" ht="44.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="0" t="s">
-        <v>1189</v>
-      </c>
-      <c r="B304" s="0" t="n">
-        <v>94596</v>
-      </c>
-      <c r="C304" s="0" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D304" s="1" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E304" s="2" t="s">
+    <row r="305" customFormat="false" ht="869.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="s">
         <v>1192</v>
       </c>
+      <c r="B305" s="0" t="n">
+        <v>91604</v>
+      </c>
+      <c r="C305" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E305" s="2" t="s">
+        <v>1195</v>
+      </c>
     </row>
-    <row r="305" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="0" t="s">
-        <v>1193</v>
-      </c>
-      <c r="B305" s="0" t="n">
-        <v>94594</v>
-      </c>
-      <c r="C305" s="0" t="s">
-        <v>1194</v>
-      </c>
-      <c r="D305" s="1" t="s">
-        <v>1195</v>
-      </c>
-      <c r="E305" s="2" t="s">
+    <row r="306" customFormat="false" ht="123.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="306" customFormat="false" ht="80.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="0" t="s">
+      <c r="B306" s="0" t="n">
+        <v>90822</v>
+      </c>
+      <c r="C306" s="0" t="s">
         <v>1197</v>
       </c>
-      <c r="B306" s="0" t="n">
-        <v>94589</v>
-      </c>
-      <c r="C306" s="0" t="s">
+      <c r="D306" s="1" t="s">
         <v>1198</v>
       </c>
-      <c r="D306" s="1" t="s">
+      <c r="E306" s="2" t="s">
         <v>1199</v>
-      </c>
-      <c r="E306" s="2" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="307" customFormat="false" ht="93.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="0" t="s">
-        <v>1201</v>
-      </c>
-      <c r="B307" s="0" t="n">
-        <v>94587</v>
-      </c>
-      <c r="C307" s="0" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D307" s="1" t="s">
-        <v>1203</v>
-      </c>
-      <c r="E307" s="2" t="s">
-        <v>1204</v>
-      </c>
-    </row>
-    <row r="308" customFormat="false" ht="58.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B308" s="0" t="n">
-        <v>94585</v>
-      </c>
-      <c r="C308" s="0" t="s">
-        <v>1206</v>
-      </c>
-      <c r="D308" s="1" t="s">
-        <v>1207</v>
-      </c>
-      <c r="E308" s="2" t="s">
-        <v>1208</v>
-      </c>
-    </row>
-    <row r="309" customFormat="false" ht="101.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="0" t="s">
-        <v>1209</v>
-      </c>
-      <c r="B309" s="0" t="n">
-        <v>94559</v>
-      </c>
-      <c r="C309" s="0" t="s">
-        <v>1210</v>
-      </c>
-      <c r="D309" s="1" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E309" s="2" t="s">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="310" customFormat="false" ht="115.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="0" t="s">
-        <v>1213</v>
-      </c>
-      <c r="B310" s="0" t="n">
-        <v>94547</v>
-      </c>
-      <c r="C310" s="0" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D310" s="1" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E310" s="2" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="311" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="0" t="s">
-        <v>1217</v>
-      </c>
-      <c r="B311" s="0" t="n">
-        <v>94540</v>
-      </c>
-      <c r="C311" s="0" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D311" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="E311" s="2" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="312" customFormat="false" ht="330.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="0" t="s">
-        <v>1221</v>
-      </c>
-      <c r="B312" s="0" t="n">
-        <v>94533</v>
-      </c>
-      <c r="C312" s="2" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D312" s="1" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E312" s="2" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="313" customFormat="false" ht="393.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="0" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B313" s="0" t="n">
-        <v>94447</v>
-      </c>
-      <c r="C313" s="0" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D313" s="1" t="s">
-        <v>1227</v>
-      </c>
-      <c r="E313" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="314" customFormat="false" ht="262.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="0" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B314" s="0" t="n">
-        <v>94412</v>
-      </c>
-      <c r="C314" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D314" s="1" t="s">
-        <v>1230</v>
-      </c>
-      <c r="E314" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="315" customFormat="false" ht="273.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="0" t="s">
-        <v>1231</v>
-      </c>
-      <c r="B315" s="0" t="n">
-        <v>94382</v>
-      </c>
-      <c r="C315" s="2" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D315" s="1" t="s">
-        <v>1233</v>
-      </c>
-      <c r="E315" s="2" t="s">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="0" t="s">
-        <v>1235</v>
-      </c>
-      <c r="B316" s="0" t="n">
-        <v>94344</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>1236</v>
-      </c>
-      <c r="E316" s="2" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="317" customFormat="false" ht="360.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="0" t="s">
-        <v>1238</v>
-      </c>
-      <c r="B317" s="0" t="n">
-        <v>94294</v>
-      </c>
-      <c r="C317" s="0" t="s">
-        <v>1239</v>
-      </c>
-      <c r="D317" s="1" t="s">
-        <v>1240</v>
-      </c>
-      <c r="E317" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="318" customFormat="false" ht="382.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="0" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B318" s="0" t="n">
-        <v>94290</v>
-      </c>
-      <c r="C318" s="0" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D318" s="1" t="s">
-        <v>1243</v>
-      </c>
-      <c r="E318" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="319" customFormat="false" ht="328.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="0" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B319" s="0" t="n">
-        <v>94287</v>
-      </c>
-      <c r="C319" s="0" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D319" s="1" t="s">
-        <v>1246</v>
-      </c>
-      <c r="E319" s="0" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="320" customFormat="false" ht="246.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="0" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B320" s="0" t="n">
-        <v>94267</v>
-      </c>
-      <c r="C320" s="0" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D320" s="1" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E320" s="2" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="0" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B321" s="0" t="n">
-        <v>94242</v>
-      </c>
-      <c r="C321" s="0" t="s">
-        <v>1252</v>
-      </c>
-      <c r="D321" s="1" t="s">
-        <v>1253</v>
-      </c>
-      <c r="E321" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="306.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="0" t="s">
-        <v>1254</v>
-      </c>
-      <c r="B322" s="0" t="n">
-        <v>94234</v>
-      </c>
-      <c r="C322" s="0" t="s">
-        <v>1255</v>
-      </c>
-      <c r="D322" s="1" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E322" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="323" customFormat="false" ht="121.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="0" t="s">
-        <v>1257</v>
-      </c>
-      <c r="B323" s="0" t="n">
-        <v>94228</v>
-      </c>
-      <c r="C323" s="0" t="s">
-        <v>1258</v>
-      </c>
-      <c r="D323" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="E323" s="0" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="324" customFormat="false" ht="869.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="0" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B324" s="0" t="n">
-        <v>91604</v>
-      </c>
-      <c r="C324" s="0" t="s">
-        <v>1261</v>
-      </c>
-      <c r="D324" s="1" t="s">
-        <v>1262</v>
-      </c>
-      <c r="E324" s="2" t="s">
-        <v>1263</v>
-      </c>
-    </row>
-    <row r="325" customFormat="false" ht="123.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="0" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B325" s="0" t="n">
-        <v>90822</v>
-      </c>
-      <c r="C325" s="0" t="s">
-        <v>1265</v>
-      </c>
-      <c r="D325" s="1" t="s">
-        <v>1266</v>
-      </c>
-      <c r="E325" s="2" t="s">
-        <v>1267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>